<commit_message>
Add calculation of actual yearly average emission decrease to backend and add result to climate-data.json
</commit_message>
<xml_diff>
--- a/data/tests/reference_dataframes/df_change_percent.xlsx
+++ b/data/tests/reference_dataframes/df_change_percent.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V291"/>
+  <dimension ref="A1:W291"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,6 +514,11 @@
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
+          <t>actualEmissionChangePercent</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
           <t>emissionChangePercent</t>
         </is>
       </c>
@@ -595,6 +600,9 @@
         </is>
       </c>
       <c r="V2" t="n">
+        <v>0.006777828626744745</v>
+      </c>
+      <c r="W2" t="n">
         <v>39.60119141410856</v>
       </c>
     </row>
@@ -675,6 +683,9 @@
         </is>
       </c>
       <c r="V3" t="n">
+        <v>-0.0287830460823655</v>
+      </c>
+      <c r="W3" t="n">
         <v>32.93073014219555</v>
       </c>
     </row>
@@ -755,6 +766,9 @@
         </is>
       </c>
       <c r="V4" t="n">
+        <v>-0.03106354699703534</v>
+      </c>
+      <c r="W4" t="n">
         <v>31.60819465943553</v>
       </c>
     </row>
@@ -835,6 +849,9 @@
         </is>
       </c>
       <c r="V5" t="n">
+        <v>-0.01574180862670948</v>
+      </c>
+      <c r="W5" t="n">
         <v>34.28459710565433</v>
       </c>
     </row>
@@ -915,6 +932,9 @@
         </is>
       </c>
       <c r="V6" t="n">
+        <v>-0.0178675368142107</v>
+      </c>
+      <c r="W6" t="n">
         <v>35.49281598445177</v>
       </c>
     </row>
@@ -995,6 +1015,9 @@
         </is>
       </c>
       <c r="V7" t="n">
+        <v>-0.05216881594416081</v>
+      </c>
+      <c r="W7" t="n">
         <v>24.16878549118003</v>
       </c>
     </row>
@@ -1075,6 +1098,9 @@
         </is>
       </c>
       <c r="V8" t="n">
+        <v>-0.01616468362625644</v>
+      </c>
+      <c r="W8" t="n">
         <v>35.05989610269589</v>
       </c>
     </row>
@@ -1155,6 +1181,9 @@
         </is>
       </c>
       <c r="V9" t="n">
+        <v>-0.01644157684384816</v>
+      </c>
+      <c r="W9" t="n">
         <v>34.11482940785217</v>
       </c>
     </row>
@@ -1235,6 +1264,9 @@
         </is>
       </c>
       <c r="V10" t="n">
+        <v>0.02436271158385382</v>
+      </c>
+      <c r="W10" t="n">
         <v>40.54794115952714</v>
       </c>
     </row>
@@ -1315,6 +1347,9 @@
         </is>
       </c>
       <c r="V11" t="n">
+        <v>-0.0009299141160527211</v>
+      </c>
+      <c r="W11" t="n">
         <v>37.31074433877556</v>
       </c>
     </row>
@@ -1395,6 +1430,9 @@
         </is>
       </c>
       <c r="V12" t="n">
+        <v>-0.01882506843830222</v>
+      </c>
+      <c r="W12" t="n">
         <v>33.76659782319905</v>
       </c>
     </row>
@@ -1475,6 +1513,9 @@
         </is>
       </c>
       <c r="V13" t="n">
+        <v>-0.08455961710818204</v>
+      </c>
+      <c r="W13" t="n">
         <v>13.70692622054494</v>
       </c>
     </row>
@@ -1555,6 +1596,9 @@
         </is>
       </c>
       <c r="V14" t="n">
+        <v>-0.01334166669638212</v>
+      </c>
+      <c r="W14" t="n">
         <v>36.30068180350944</v>
       </c>
     </row>
@@ -1635,6 +1679,9 @@
         </is>
       </c>
       <c r="V15" t="n">
+        <v>-0.04490451877030514</v>
+      </c>
+      <c r="W15" t="n">
         <v>26.29282134492055</v>
       </c>
     </row>
@@ -1715,6 +1762,9 @@
         </is>
       </c>
       <c r="V16" t="n">
+        <v>0.02845237355137667</v>
+      </c>
+      <c r="W16" t="n">
         <v>43.81761777061995</v>
       </c>
     </row>
@@ -1795,6 +1845,9 @@
         </is>
       </c>
       <c r="V17" t="n">
+        <v>0.0004800095132785536</v>
+      </c>
+      <c r="W17" t="n">
         <v>38.77623936364633</v>
       </c>
     </row>
@@ -1875,6 +1928,9 @@
         </is>
       </c>
       <c r="V18" t="n">
+        <v>-0.0198036971037208</v>
+      </c>
+      <c r="W18" t="n">
         <v>32.82712926687659</v>
       </c>
     </row>
@@ -1955,6 +2011,9 @@
         </is>
       </c>
       <c r="V19" t="n">
+        <v>-0.03134109373275062</v>
+      </c>
+      <c r="W19" t="n">
         <v>32.5284339779548</v>
       </c>
     </row>
@@ -2035,6 +2094,9 @@
         </is>
       </c>
       <c r="V20" t="n">
+        <v>-0.01812206297325211</v>
+      </c>
+      <c r="W20" t="n">
         <v>33.6513579601908</v>
       </c>
     </row>
@@ -2115,6 +2177,9 @@
         </is>
       </c>
       <c r="V21" t="n">
+        <v>-0.02186800053113524</v>
+      </c>
+      <c r="W21" t="n">
         <v>33.47734245979111</v>
       </c>
     </row>
@@ -2195,6 +2260,9 @@
         </is>
       </c>
       <c r="V22" t="n">
+        <v>-0.04366957800173508</v>
+      </c>
+      <c r="W22" t="n">
         <v>29.0381998336958</v>
       </c>
     </row>
@@ -2275,6 +2343,9 @@
         </is>
       </c>
       <c r="V23" t="n">
+        <v>-0.01357684952033877</v>
+      </c>
+      <c r="W23" t="n">
         <v>30.99868819219974</v>
       </c>
     </row>
@@ -2355,6 +2426,9 @@
         </is>
       </c>
       <c r="V24" t="n">
+        <v>-0.01854131169923561</v>
+      </c>
+      <c r="W24" t="n">
         <v>34.23402310317982</v>
       </c>
     </row>
@@ -2435,6 +2509,9 @@
         </is>
       </c>
       <c r="V25" t="n">
+        <v>-0.05591413142280759</v>
+      </c>
+      <c r="W25" t="n">
         <v>26.27688609604742</v>
       </c>
     </row>
@@ -2515,6 +2592,9 @@
         </is>
       </c>
       <c r="V26" t="n">
+        <v>-0.06208913878116392</v>
+      </c>
+      <c r="W26" t="n">
         <v>24.92880315588712</v>
       </c>
     </row>
@@ -2595,6 +2675,9 @@
         </is>
       </c>
       <c r="V27" t="n">
+        <v>-0.03300449527495998</v>
+      </c>
+      <c r="W27" t="n">
         <v>31.48644646455086</v>
       </c>
     </row>
@@ -2675,6 +2758,9 @@
         </is>
       </c>
       <c r="V28" t="n">
+        <v>-0.02638673933704393</v>
+      </c>
+      <c r="W28" t="n">
         <v>32.21986665387803</v>
       </c>
     </row>
@@ -2755,6 +2841,9 @@
         </is>
       </c>
       <c r="V29" t="n">
+        <v>-0.07708244076836777</v>
+      </c>
+      <c r="W29" t="n">
         <v>17.94296683967403</v>
       </c>
     </row>
@@ -2835,6 +2924,9 @@
         </is>
       </c>
       <c r="V30" t="n">
+        <v>-0.01354991645079016</v>
+      </c>
+      <c r="W30" t="n">
         <v>35.41310928770709</v>
       </c>
     </row>
@@ -2915,6 +3007,9 @@
         </is>
       </c>
       <c r="V31" t="n">
+        <v>-0.002846718397882009</v>
+      </c>
+      <c r="W31" t="n">
         <v>39.25064714419205</v>
       </c>
     </row>
@@ -2995,6 +3090,9 @@
         </is>
       </c>
       <c r="V32" t="n">
+        <v>0.00225454562032365</v>
+      </c>
+      <c r="W32" t="n">
         <v>37.36256336184437</v>
       </c>
     </row>
@@ -3075,6 +3173,9 @@
         </is>
       </c>
       <c r="V33" t="n">
+        <v>-0.02400142801543735</v>
+      </c>
+      <c r="W33" t="n">
         <v>32.39746063225301</v>
       </c>
     </row>
@@ -3155,6 +3256,9 @@
         </is>
       </c>
       <c r="V34" t="n">
+        <v>-0.01350995714705207</v>
+      </c>
+      <c r="W34" t="n">
         <v>34.08219737936341</v>
       </c>
     </row>
@@ -3235,6 +3339,9 @@
         </is>
       </c>
       <c r="V35" t="n">
+        <v>-0.03045889830955396</v>
+      </c>
+      <c r="W35" t="n">
         <v>31.65319593487783</v>
       </c>
     </row>
@@ -3315,6 +3422,9 @@
         </is>
       </c>
       <c r="V36" t="n">
+        <v>-0.02986809321984917</v>
+      </c>
+      <c r="W36" t="n">
         <v>32.69265428871601</v>
       </c>
     </row>
@@ -3395,6 +3505,9 @@
         </is>
       </c>
       <c r="V37" t="n">
+        <v>-0.01740867144413108</v>
+      </c>
+      <c r="W37" t="n">
         <v>32.59089728610387</v>
       </c>
     </row>
@@ -3475,6 +3588,9 @@
         </is>
       </c>
       <c r="V38" t="n">
+        <v>0.02298358801111555</v>
+      </c>
+      <c r="W38" t="n">
         <v>39.51601622033161</v>
       </c>
     </row>
@@ -3555,6 +3671,9 @@
         </is>
       </c>
       <c r="V39" t="n">
+        <v>-0.0421463226731227</v>
+      </c>
+      <c r="W39" t="n">
         <v>28.91387434890832</v>
       </c>
     </row>
@@ -3635,6 +3754,9 @@
         </is>
       </c>
       <c r="V40" t="n">
+        <v>-0.05041666001765694</v>
+      </c>
+      <c r="W40" t="n">
         <v>26.29469056440499</v>
       </c>
     </row>
@@ -3715,6 +3837,9 @@
         </is>
       </c>
       <c r="V41" t="n">
+        <v>-0.01228741410836448</v>
+      </c>
+      <c r="W41" t="n">
         <v>35.35846257474203</v>
       </c>
     </row>
@@ -3795,6 +3920,9 @@
         </is>
       </c>
       <c r="V42" t="n">
+        <v>-0.02999395400694676</v>
+      </c>
+      <c r="W42" t="n">
         <v>32.09721105161999</v>
       </c>
     </row>
@@ -3875,6 +4003,9 @@
         </is>
       </c>
       <c r="V43" t="n">
+        <v>-0.0468683423515194</v>
+      </c>
+      <c r="W43" t="n">
         <v>27.06572172035454</v>
       </c>
     </row>
@@ -3955,6 +4086,9 @@
         </is>
       </c>
       <c r="V44" t="n">
+        <v>-0.0274852132459015</v>
+      </c>
+      <c r="W44" t="n">
         <v>32.77526244267153</v>
       </c>
     </row>
@@ -4035,6 +4169,9 @@
         </is>
       </c>
       <c r="V45" t="n">
+        <v>-0.018006322130368</v>
+      </c>
+      <c r="W45" t="n">
         <v>34.17978994905047</v>
       </c>
     </row>
@@ -4115,6 +4252,9 @@
         </is>
       </c>
       <c r="V46" t="n">
+        <v>-0.03943157449362941</v>
+      </c>
+      <c r="W46" t="n">
         <v>29.72478349564166</v>
       </c>
     </row>
@@ -4195,6 +4335,9 @@
         </is>
       </c>
       <c r="V47" t="n">
+        <v>-0.0286441362096813</v>
+      </c>
+      <c r="W47" t="n">
         <v>31.57293868110329</v>
       </c>
     </row>
@@ -4275,6 +4418,9 @@
         </is>
       </c>
       <c r="V48" t="n">
+        <v>-0.01212789555846249</v>
+      </c>
+      <c r="W48" t="n">
         <v>36.85881033638594</v>
       </c>
     </row>
@@ -4355,6 +4501,9 @@
         </is>
       </c>
       <c r="V49" t="n">
+        <v>-0.04541812620417315</v>
+      </c>
+      <c r="W49" t="n">
         <v>28.46158836293336</v>
       </c>
     </row>
@@ -4435,6 +4584,9 @@
         </is>
       </c>
       <c r="V50" t="n">
+        <v>-0.03608168816305118</v>
+      </c>
+      <c r="W50" t="n">
         <v>30.42055138785142</v>
       </c>
     </row>
@@ -4515,6 +4667,9 @@
         </is>
       </c>
       <c r="V51" t="n">
+        <v>-0.06285360315497887</v>
+      </c>
+      <c r="W51" t="n">
         <v>22.8231984415254</v>
       </c>
     </row>
@@ -4595,6 +4750,9 @@
         </is>
       </c>
       <c r="V52" t="n">
+        <v>-0.04973028472009036</v>
+      </c>
+      <c r="W52" t="n">
         <v>27.04935891881998</v>
       </c>
     </row>
@@ -4675,6 +4833,9 @@
         </is>
       </c>
       <c r="V53" t="n">
+        <v>-0.05474915172472286</v>
+      </c>
+      <c r="W53" t="n">
         <v>27.93561704728159</v>
       </c>
     </row>
@@ -4755,6 +4916,9 @@
         </is>
       </c>
       <c r="V54" t="n">
+        <v>-0.00332881034127633</v>
+      </c>
+      <c r="W54" t="n">
         <v>39.08604544949362</v>
       </c>
     </row>
@@ -4835,6 +4999,9 @@
         </is>
       </c>
       <c r="V55" t="n">
+        <v>-0.02327162842700123</v>
+      </c>
+      <c r="W55" t="n">
         <v>33.54018170983478</v>
       </c>
     </row>
@@ -4915,6 +5082,9 @@
         </is>
       </c>
       <c r="V56" t="n">
+        <v>-0.02958353319528445</v>
+      </c>
+      <c r="W56" t="n">
         <v>31.97839758985122</v>
       </c>
     </row>
@@ -4995,6 +5165,9 @@
         </is>
       </c>
       <c r="V57" t="n">
+        <v>0.02076850573416765</v>
+      </c>
+      <c r="W57" t="n">
         <v>41.86913904613861</v>
       </c>
     </row>
@@ -5075,6 +5248,9 @@
         </is>
       </c>
       <c r="V58" t="n">
+        <v>-0.03145322305546139</v>
+      </c>
+      <c r="W58" t="n">
         <v>31.21333724150885</v>
       </c>
     </row>
@@ -5155,6 +5331,9 @@
         </is>
       </c>
       <c r="V59" t="n">
+        <v>-0.007470653488961477</v>
+      </c>
+      <c r="W59" t="n">
         <v>34.81861664270994</v>
       </c>
     </row>
@@ -5235,6 +5414,9 @@
         </is>
       </c>
       <c r="V60" t="n">
+        <v>0.002828487744895252</v>
+      </c>
+      <c r="W60" t="n">
         <v>37.21889256446094</v>
       </c>
     </row>
@@ -5315,6 +5497,9 @@
         </is>
       </c>
       <c r="V61" t="n">
+        <v>-0.002990868784666925</v>
+      </c>
+      <c r="W61" t="n">
         <v>37.32152661308202</v>
       </c>
     </row>
@@ -5395,6 +5580,9 @@
         </is>
       </c>
       <c r="V62" t="n">
+        <v>-0.004256575094313014</v>
+      </c>
+      <c r="W62" t="n">
         <v>35.18970249025502</v>
       </c>
     </row>
@@ -5475,6 +5663,9 @@
         </is>
       </c>
       <c r="V63" t="n">
+        <v>-0.03380060367640274</v>
+      </c>
+      <c r="W63" t="n">
         <v>30.80460642460513</v>
       </c>
     </row>
@@ -5555,6 +5746,9 @@
         </is>
       </c>
       <c r="V64" t="n">
+        <v>-0.01208913283707802</v>
+      </c>
+      <c r="W64" t="n">
         <v>36.31882773467608</v>
       </c>
     </row>
@@ -5635,6 +5829,9 @@
         </is>
       </c>
       <c r="V65" t="n">
+        <v>-0.01721516085117787</v>
+      </c>
+      <c r="W65" t="n">
         <v>33.70275223442906</v>
       </c>
     </row>
@@ -5715,6 +5912,9 @@
         </is>
       </c>
       <c r="V66" t="n">
+        <v>-0.0244554722484178</v>
+      </c>
+      <c r="W66" t="n">
         <v>31.84305630424471</v>
       </c>
     </row>
@@ -5795,6 +5995,9 @@
         </is>
       </c>
       <c r="V67" t="n">
+        <v>-0.04156891058175606</v>
+      </c>
+      <c r="W67" t="n">
         <v>30.00080702616452</v>
       </c>
     </row>
@@ -5875,6 +6078,9 @@
         </is>
       </c>
       <c r="V68" t="n">
+        <v>-0.02227015185260305</v>
+      </c>
+      <c r="W68" t="n">
         <v>34.78105894943292</v>
       </c>
     </row>
@@ -5955,6 +6161,9 @@
         </is>
       </c>
       <c r="V69" t="n">
+        <v>-0.0367929949312857</v>
+      </c>
+      <c r="W69" t="n">
         <v>29.4442253288391</v>
       </c>
     </row>
@@ -6035,6 +6244,9 @@
         </is>
       </c>
       <c r="V70" t="n">
+        <v>0.009813313647620255</v>
+      </c>
+      <c r="W70" t="n">
         <v>41.17654967368468</v>
       </c>
     </row>
@@ -6115,6 +6327,9 @@
         </is>
       </c>
       <c r="V71" t="n">
+        <v>-0.01426433068648687</v>
+      </c>
+      <c r="W71" t="n">
         <v>35.70109756028919</v>
       </c>
     </row>
@@ -6195,6 +6410,9 @@
         </is>
       </c>
       <c r="V72" t="n">
+        <v>-0.03276840816968993</v>
+      </c>
+      <c r="W72" t="n">
         <v>30.99203559202281</v>
       </c>
     </row>
@@ -6275,6 +6493,9 @@
         </is>
       </c>
       <c r="V73" t="n">
+        <v>-0.03337975198679622</v>
+      </c>
+      <c r="W73" t="n">
         <v>31.18548721928247</v>
       </c>
     </row>
@@ -6355,6 +6576,9 @@
         </is>
       </c>
       <c r="V74" t="n">
+        <v>-0.02632062844398159</v>
+      </c>
+      <c r="W74" t="n">
         <v>28.77470219880741</v>
       </c>
     </row>
@@ -6435,6 +6659,9 @@
         </is>
       </c>
       <c r="V75" t="n">
+        <v>-0.04102879391489345</v>
+      </c>
+      <c r="W75" t="n">
         <v>29.66007465652061</v>
       </c>
     </row>
@@ -6515,6 +6742,9 @@
         </is>
       </c>
       <c r="V76" t="n">
+        <v>-0.03615269057138866</v>
+      </c>
+      <c r="W76" t="n">
         <v>29.18485296883964</v>
       </c>
     </row>
@@ -6595,6 +6825,9 @@
         </is>
       </c>
       <c r="V77" t="n">
+        <v>-0.0311447190759423</v>
+      </c>
+      <c r="W77" t="n">
         <v>31.57636963159134</v>
       </c>
     </row>
@@ -6675,6 +6908,9 @@
         </is>
       </c>
       <c r="V78" t="n">
+        <v>-0.02111506089788784</v>
+      </c>
+      <c r="W78" t="n">
         <v>31.82191010359449</v>
       </c>
     </row>
@@ -6755,6 +6991,9 @@
         </is>
       </c>
       <c r="V79" t="n">
+        <v>-0.03145866745714621</v>
+      </c>
+      <c r="W79" t="n">
         <v>30.30990793487499</v>
       </c>
     </row>
@@ -6835,6 +7074,9 @@
         </is>
       </c>
       <c r="V80" t="n">
+        <v>-0.1014531115188736</v>
+      </c>
+      <c r="W80" t="n">
         <v>6.72541151250168</v>
       </c>
     </row>
@@ -6915,6 +7157,9 @@
         </is>
       </c>
       <c r="V81" t="n">
+        <v>-0.04110568386525486</v>
+      </c>
+      <c r="W81" t="n">
         <v>29.36718109192282</v>
       </c>
     </row>
@@ -6995,6 +7240,9 @@
         </is>
       </c>
       <c r="V82" t="n">
+        <v>-0.01374657364152947</v>
+      </c>
+      <c r="W82" t="n">
         <v>36.14111844273287</v>
       </c>
     </row>
@@ -7075,6 +7323,9 @@
         </is>
       </c>
       <c r="V83" t="n">
+        <v>-0.01418292510141253</v>
+      </c>
+      <c r="W83" t="n">
         <v>37.21412700248587</v>
       </c>
     </row>
@@ -7155,6 +7406,9 @@
         </is>
       </c>
       <c r="V84" t="n">
+        <v>-0.01471693880674202</v>
+      </c>
+      <c r="W84" t="n">
         <v>35.13131315028622</v>
       </c>
     </row>
@@ -7235,6 +7489,9 @@
         </is>
       </c>
       <c r="V85" t="n">
+        <v>0.004868331369381936</v>
+      </c>
+      <c r="W85" t="n">
         <v>36.57493442511435</v>
       </c>
     </row>
@@ -7315,6 +7572,9 @@
         </is>
       </c>
       <c r="V86" t="n">
+        <v>-0.04254629183408467</v>
+      </c>
+      <c r="W86" t="n">
         <v>26.82962418910139</v>
       </c>
     </row>
@@ -7395,6 +7655,9 @@
         </is>
       </c>
       <c r="V87" t="n">
+        <v>-0.02016528738371191</v>
+      </c>
+      <c r="W87" t="n">
         <v>34.57727749901252</v>
       </c>
     </row>
@@ -7475,6 +7738,9 @@
         </is>
       </c>
       <c r="V88" t="n">
+        <v>-0.03210717808799588</v>
+      </c>
+      <c r="W88" t="n">
         <v>31.65209348130818</v>
       </c>
     </row>
@@ -7555,6 +7821,9 @@
         </is>
       </c>
       <c r="V89" t="n">
+        <v>-0.05030681936292775</v>
+      </c>
+      <c r="W89" t="n">
         <v>25.82557308017028</v>
       </c>
     </row>
@@ -7635,6 +7904,9 @@
         </is>
       </c>
       <c r="V90" t="n">
+        <v>-0.008037628370891697</v>
+      </c>
+      <c r="W90" t="n">
         <v>36.53162107041114</v>
       </c>
     </row>
@@ -7715,6 +7987,9 @@
         </is>
       </c>
       <c r="V91" t="n">
+        <v>-0.02130192011128492</v>
+      </c>
+      <c r="W91" t="n">
         <v>34.49956836862127</v>
       </c>
     </row>
@@ -7795,6 +8070,9 @@
         </is>
       </c>
       <c r="V92" t="n">
+        <v>-0.01108513356388517</v>
+      </c>
+      <c r="W92" t="n">
         <v>35.28217674836681</v>
       </c>
     </row>
@@ -7875,6 +8153,9 @@
         </is>
       </c>
       <c r="V93" t="n">
+        <v>-0.03907611830891281</v>
+      </c>
+      <c r="W93" t="n">
         <v>29.22572405674112</v>
       </c>
     </row>
@@ -7955,6 +8236,9 @@
         </is>
       </c>
       <c r="V94" t="n">
+        <v>-0.04118019672572016</v>
+      </c>
+      <c r="W94" t="n">
         <v>28.36854324784929</v>
       </c>
     </row>
@@ -8035,6 +8319,9 @@
         </is>
       </c>
       <c r="V95" t="n">
+        <v>0.1148996346141485</v>
+      </c>
+      <c r="W95" t="n">
         <v>47.85580233640622</v>
       </c>
     </row>
@@ -8115,6 +8402,9 @@
         </is>
       </c>
       <c r="V96" t="n">
+        <v>-0.0287515697748225</v>
+      </c>
+      <c r="W96" t="n">
         <v>30.79459706493006</v>
       </c>
     </row>
@@ -8195,6 +8485,9 @@
         </is>
       </c>
       <c r="V97" t="n">
+        <v>-0.02522742820392277</v>
+      </c>
+      <c r="W97" t="n">
         <v>33.68561151646555</v>
       </c>
     </row>
@@ -8275,6 +8568,9 @@
         </is>
       </c>
       <c r="V98" t="n">
+        <v>-0.01857507519234883</v>
+      </c>
+      <c r="W98" t="n">
         <v>33.96430222705212</v>
       </c>
     </row>
@@ -8355,6 +8651,9 @@
         </is>
       </c>
       <c r="V99" t="n">
+        <v>-0.03103461539061256</v>
+      </c>
+      <c r="W99" t="n">
         <v>31.35004602107368</v>
       </c>
     </row>
@@ -8435,6 +8734,9 @@
         </is>
       </c>
       <c r="V100" t="n">
+        <v>-0.005733871366737643</v>
+      </c>
+      <c r="W100" t="n">
         <v>36.26384951474642</v>
       </c>
     </row>
@@ -8515,6 +8817,9 @@
         </is>
       </c>
       <c r="V101" t="n">
+        <v>-0.03585364809220387</v>
+      </c>
+      <c r="W101" t="n">
         <v>30.17798081373127</v>
       </c>
     </row>
@@ -8595,6 +8900,9 @@
         </is>
       </c>
       <c r="V102" t="n">
+        <v>0.00422125687756205</v>
+      </c>
+      <c r="W102" t="n">
         <v>39.09472937072151</v>
       </c>
     </row>
@@ -8675,6 +8983,9 @@
         </is>
       </c>
       <c r="V103" t="n">
+        <v>-0.02363863138643421</v>
+      </c>
+      <c r="W103" t="n">
         <v>33.46785750789208</v>
       </c>
     </row>
@@ -8755,6 +9066,9 @@
         </is>
       </c>
       <c r="V104" t="n">
+        <v>-0.03028610367101815</v>
+      </c>
+      <c r="W104" t="n">
         <v>31.91856755078927</v>
       </c>
     </row>
@@ -8835,6 +9149,9 @@
         </is>
       </c>
       <c r="V105" t="n">
+        <v>-0.01668535266178965</v>
+      </c>
+      <c r="W105" t="n">
         <v>32.94251333012927</v>
       </c>
     </row>
@@ -8915,6 +9232,9 @@
         </is>
       </c>
       <c r="V106" t="n">
+        <v>-0.03440699875481342</v>
+      </c>
+      <c r="W106" t="n">
         <v>31.6225105519062</v>
       </c>
     </row>
@@ -8995,6 +9315,9 @@
         </is>
       </c>
       <c r="V107" t="n">
+        <v>-0.03405073736539824</v>
+      </c>
+      <c r="W107" t="n">
         <v>31.18057150165529</v>
       </c>
     </row>
@@ -9075,6 +9398,9 @@
         </is>
       </c>
       <c r="V108" t="n">
+        <v>-0.06443699806862473</v>
+      </c>
+      <c r="W108" t="n">
         <v>21.25177688787407</v>
       </c>
     </row>
@@ -9155,6 +9481,9 @@
         </is>
       </c>
       <c r="V109" t="n">
+        <v>0.002305479351703594</v>
+      </c>
+      <c r="W109" t="n">
         <v>37.0114566395333</v>
       </c>
     </row>
@@ -9235,6 +9564,9 @@
         </is>
       </c>
       <c r="V110" t="n">
+        <v>-0.02521882051041456</v>
+      </c>
+      <c r="W110" t="n">
         <v>33.3840070465324</v>
       </c>
     </row>
@@ -9315,6 +9647,9 @@
         </is>
       </c>
       <c r="V111" t="n">
+        <v>-0.01848249590153418</v>
+      </c>
+      <c r="W111" t="n">
         <v>34.64837214460356</v>
       </c>
     </row>
@@ -9395,6 +9730,9 @@
         </is>
       </c>
       <c r="V112" t="n">
+        <v>-0.0177916276418841</v>
+      </c>
+      <c r="W112" t="n">
         <v>35.12206163185168</v>
       </c>
     </row>
@@ -9475,6 +9813,9 @@
         </is>
       </c>
       <c r="V113" t="n">
+        <v>-0.02712950512199258</v>
+      </c>
+      <c r="W113" t="n">
         <v>32.84242237264701</v>
       </c>
     </row>
@@ -9555,6 +9896,9 @@
         </is>
       </c>
       <c r="V114" t="n">
+        <v>-0.01868945577905195</v>
+      </c>
+      <c r="W114" t="n">
         <v>31.95078786072603</v>
       </c>
     </row>
@@ -9635,6 +9979,9 @@
         </is>
       </c>
       <c r="V115" t="n">
+        <v>-0.04442915307396002</v>
+      </c>
+      <c r="W115" t="n">
         <v>28.52693695435341</v>
       </c>
     </row>
@@ -9715,6 +10062,9 @@
         </is>
       </c>
       <c r="V116" t="n">
+        <v>-0.009288361236154856</v>
+      </c>
+      <c r="W116" t="n">
         <v>36.73157166028878</v>
       </c>
     </row>
@@ -9795,6 +10145,9 @@
         </is>
       </c>
       <c r="V117" t="n">
+        <v>-0.03148634275252381</v>
+      </c>
+      <c r="W117" t="n">
         <v>32.55324697981289</v>
       </c>
     </row>
@@ -9875,6 +10228,9 @@
         </is>
       </c>
       <c r="V118" t="n">
+        <v>-0.0210608140685666</v>
+      </c>
+      <c r="W118" t="n">
         <v>34.37877322248394</v>
       </c>
     </row>
@@ -9955,6 +10311,9 @@
         </is>
       </c>
       <c r="V119" t="n">
+        <v>-0.03742913095904383</v>
+      </c>
+      <c r="W119" t="n">
         <v>29.68019126937816</v>
       </c>
     </row>
@@ -10035,6 +10394,9 @@
         </is>
       </c>
       <c r="V120" t="n">
+        <v>-0.04606428745614561</v>
+      </c>
+      <c r="W120" t="n">
         <v>27.70758000799979</v>
       </c>
     </row>
@@ -10115,6 +10477,9 @@
         </is>
       </c>
       <c r="V121" t="n">
+        <v>-0.03019107506715167</v>
+      </c>
+      <c r="W121" t="n">
         <v>31.21117253890304</v>
       </c>
     </row>
@@ -10195,6 +10560,9 @@
         </is>
       </c>
       <c r="V122" t="n">
+        <v>0.03599976466170274</v>
+      </c>
+      <c r="W122" t="n">
         <v>42.42317164225275</v>
       </c>
     </row>
@@ -10275,6 +10643,9 @@
         </is>
       </c>
       <c r="V123" t="n">
+        <v>-0.02784243261187225</v>
+      </c>
+      <c r="W123" t="n">
         <v>33.27220919540804</v>
       </c>
     </row>
@@ -10355,6 +10726,9 @@
         </is>
       </c>
       <c r="V124" t="n">
+        <v>-0.003230681739759642</v>
+      </c>
+      <c r="W124" t="n">
         <v>38.34817437753129</v>
       </c>
     </row>
@@ -10435,6 +10809,9 @@
         </is>
       </c>
       <c r="V125" t="n">
+        <v>-0.01086784161136056</v>
+      </c>
+      <c r="W125" t="n">
         <v>33.66396681805799</v>
       </c>
     </row>
@@ -10515,6 +10892,9 @@
         </is>
       </c>
       <c r="V126" t="n">
+        <v>-0.006990999729136958</v>
+      </c>
+      <c r="W126" t="n">
         <v>35.39891062154671</v>
       </c>
     </row>
@@ -10595,6 +10975,9 @@
         </is>
       </c>
       <c r="V127" t="n">
+        <v>-0.03395600549502172</v>
+      </c>
+      <c r="W127" t="n">
         <v>30.53479534318902</v>
       </c>
     </row>
@@ -10675,6 +11058,9 @@
         </is>
       </c>
       <c r="V128" t="n">
+        <v>-0.05406403533281193</v>
+      </c>
+      <c r="W128" t="n">
         <v>27.0381797410077</v>
       </c>
     </row>
@@ -10755,6 +11141,9 @@
         </is>
       </c>
       <c r="V129" t="n">
+        <v>-0.05759797618256795</v>
+      </c>
+      <c r="W129" t="n">
         <v>25.56496370928047</v>
       </c>
     </row>
@@ -10835,6 +11224,9 @@
         </is>
       </c>
       <c r="V130" t="n">
+        <v>-0.0309762647083019</v>
+      </c>
+      <c r="W130" t="n">
         <v>31.63941919339069</v>
       </c>
     </row>
@@ -10915,6 +11307,9 @@
         </is>
       </c>
       <c r="V131" t="n">
+        <v>-0.06931295608440081</v>
+      </c>
+      <c r="W131" t="n">
         <v>21.65718932773737</v>
       </c>
     </row>
@@ -10995,6 +11390,9 @@
         </is>
       </c>
       <c r="V132" t="n">
+        <v>0.04552326517363181</v>
+      </c>
+      <c r="W132" t="n">
         <v>40.31061552061322</v>
       </c>
     </row>
@@ -11075,6 +11473,9 @@
         </is>
       </c>
       <c r="V133" t="n">
+        <v>-0.04502774001772303</v>
+      </c>
+      <c r="W133" t="n">
         <v>29.37847848325799</v>
       </c>
     </row>
@@ -11155,6 +11556,9 @@
         </is>
       </c>
       <c r="V134" t="n">
+        <v>-0.02734785362508843</v>
+      </c>
+      <c r="W134" t="n">
         <v>31.54728943584016</v>
       </c>
     </row>
@@ -11235,6 +11639,9 @@
         </is>
       </c>
       <c r="V135" t="n">
+        <v>0.01898382752412984</v>
+      </c>
+      <c r="W135" t="n">
         <v>33.19793710941376</v>
       </c>
     </row>
@@ -11315,6 +11722,9 @@
         </is>
       </c>
       <c r="V136" t="n">
+        <v>-0.06899481889017173</v>
+      </c>
+      <c r="W136" t="n">
         <v>21.02199837965129</v>
       </c>
     </row>
@@ -11395,6 +11805,9 @@
         </is>
       </c>
       <c r="V137" t="n">
+        <v>-0.04310070850655964</v>
+      </c>
+      <c r="W137" t="n">
         <v>27.35231960414826</v>
       </c>
     </row>
@@ -11475,6 +11888,9 @@
         </is>
       </c>
       <c r="V138" t="n">
+        <v>-0.0164586810145942</v>
+      </c>
+      <c r="W138" t="n">
         <v>34.55283916910116</v>
       </c>
     </row>
@@ -11555,6 +11971,9 @@
         </is>
       </c>
       <c r="V139" t="n">
+        <v>-0.02764640954505996</v>
+      </c>
+      <c r="W139" t="n">
         <v>33.51472544762627</v>
       </c>
     </row>
@@ -11635,6 +12054,9 @@
         </is>
       </c>
       <c r="V140" t="n">
+        <v>-0.02534981451406505</v>
+      </c>
+      <c r="W140" t="n">
         <v>32.62002687127777</v>
       </c>
     </row>
@@ -11715,6 +12137,9 @@
         </is>
       </c>
       <c r="V141" t="n">
+        <v>-0.02657942111156249</v>
+      </c>
+      <c r="W141" t="n">
         <v>33.35512156409515</v>
       </c>
     </row>
@@ -11795,6 +12220,9 @@
         </is>
       </c>
       <c r="V142" t="n">
+        <v>-0.02986450045122585</v>
+      </c>
+      <c r="W142" t="n">
         <v>32.11476176938478</v>
       </c>
     </row>
@@ -11875,6 +12303,9 @@
         </is>
       </c>
       <c r="V143" t="n">
+        <v>-0.02818304617776572</v>
+      </c>
+      <c r="W143" t="n">
         <v>32.84080961377024</v>
       </c>
     </row>
@@ -11955,6 +12386,9 @@
         </is>
       </c>
       <c r="V144" t="n">
+        <v>-0.03528169608249762</v>
+      </c>
+      <c r="W144" t="n">
         <v>30.37949879057129</v>
       </c>
     </row>
@@ -12035,6 +12469,9 @@
         </is>
       </c>
       <c r="V145" t="n">
+        <v>-0.03659748489437211</v>
+      </c>
+      <c r="W145" t="n">
         <v>29.98523642102252</v>
       </c>
     </row>
@@ -12115,6 +12552,9 @@
         </is>
       </c>
       <c r="V146" t="n">
+        <v>-0.02060444643347544</v>
+      </c>
+      <c r="W146" t="n">
         <v>34.10882844891942</v>
       </c>
     </row>
@@ -12195,6 +12635,9 @@
         </is>
       </c>
       <c r="V147" t="n">
+        <v>0.03145420963154026</v>
+      </c>
+      <c r="W147" t="n">
         <v>38.81864983798778</v>
       </c>
     </row>
@@ -12275,6 +12718,9 @@
         </is>
       </c>
       <c r="V148" t="n">
+        <v>-0.04501834533211457</v>
+      </c>
+      <c r="W148" t="n">
         <v>28.30737536214323</v>
       </c>
     </row>
@@ -12355,6 +12801,9 @@
         </is>
       </c>
       <c r="V149" t="n">
+        <v>-0.03083488915064071</v>
+      </c>
+      <c r="W149" t="n">
         <v>30.14103794311502</v>
       </c>
     </row>
@@ -12435,6 +12884,9 @@
         </is>
       </c>
       <c r="V150" t="n">
+        <v>-0.03659171907563687</v>
+      </c>
+      <c r="W150" t="n">
         <v>27.67309734383133</v>
       </c>
     </row>
@@ -12515,6 +12967,9 @@
         </is>
       </c>
       <c r="V151" t="n">
+        <v>0.00214792330784494</v>
+      </c>
+      <c r="W151" t="n">
         <v>36.77230926866545</v>
       </c>
     </row>
@@ -12595,6 +13050,9 @@
         </is>
       </c>
       <c r="V152" t="n">
+        <v>-0.01997278961361583</v>
+      </c>
+      <c r="W152" t="n">
         <v>34.29161397166256</v>
       </c>
     </row>
@@ -12675,6 +13133,9 @@
         </is>
       </c>
       <c r="V153" t="n">
+        <v>-0.04139151439220543</v>
+      </c>
+      <c r="W153" t="n">
         <v>28.67394936909493</v>
       </c>
     </row>
@@ -12755,6 +13216,9 @@
         </is>
       </c>
       <c r="V154" t="n">
+        <v>-0.04341970438623122</v>
+      </c>
+      <c r="W154" t="n">
         <v>29.46416774344108</v>
       </c>
     </row>
@@ -12835,6 +13299,9 @@
         </is>
       </c>
       <c r="V155" t="n">
+        <v>-0.04020381496905393</v>
+      </c>
+      <c r="W155" t="n">
         <v>29.4646010730076</v>
       </c>
     </row>
@@ -12915,6 +13382,9 @@
         </is>
       </c>
       <c r="V156" t="n">
+        <v>-0.008945756862743416</v>
+      </c>
+      <c r="W156" t="n">
         <v>35.70419232505186</v>
       </c>
     </row>
@@ -12995,6 +13465,9 @@
         </is>
       </c>
       <c r="V157" t="n">
+        <v>-0.008233307650047372</v>
+      </c>
+      <c r="W157" t="n">
         <v>35.5206326911991</v>
       </c>
     </row>
@@ -13075,6 +13548,9 @@
         </is>
       </c>
       <c r="V158" t="n">
+        <v>-0.02455567627195859</v>
+      </c>
+      <c r="W158" t="n">
         <v>33.02763958828459</v>
       </c>
     </row>
@@ -13155,6 +13631,9 @@
         </is>
       </c>
       <c r="V159" t="n">
+        <v>-0.05351724292924414</v>
+      </c>
+      <c r="W159" t="n">
         <v>27.26282840216225</v>
       </c>
     </row>
@@ -13235,6 +13714,9 @@
         </is>
       </c>
       <c r="V160" t="n">
+        <v>0.02847113011932829</v>
+      </c>
+      <c r="W160" t="n">
         <v>40.30002428787438</v>
       </c>
     </row>
@@ -13315,6 +13797,9 @@
         </is>
       </c>
       <c r="V161" t="n">
+        <v>-0.02255101327389643</v>
+      </c>
+      <c r="W161" t="n">
         <v>33.06647677680973</v>
       </c>
     </row>
@@ -13395,6 +13880,9 @@
         </is>
       </c>
       <c r="V162" t="n">
+        <v>-0.01908561809193959</v>
+      </c>
+      <c r="W162" t="n">
         <v>35.04939909600674</v>
       </c>
     </row>
@@ -13475,6 +13963,9 @@
         </is>
       </c>
       <c r="V163" t="n">
+        <v>-0.02743682577517599</v>
+      </c>
+      <c r="W163" t="n">
         <v>29.64261365716365</v>
       </c>
     </row>
@@ -13555,6 +14046,9 @@
         </is>
       </c>
       <c r="V164" t="n">
+        <v>-0.0229931779358363</v>
+      </c>
+      <c r="W164" t="n">
         <v>32.61865483828312</v>
       </c>
     </row>
@@ -13635,6 +14129,9 @@
         </is>
       </c>
       <c r="V165" t="n">
+        <v>-0.06407084894383386</v>
+      </c>
+      <c r="W165" t="n">
         <v>23.49996416411781</v>
       </c>
     </row>
@@ -13715,6 +14212,9 @@
         </is>
       </c>
       <c r="V166" t="n">
+        <v>-0.02622716034918423</v>
+      </c>
+      <c r="W166" t="n">
         <v>31.56483774685117</v>
       </c>
     </row>
@@ -13795,6 +14295,9 @@
         </is>
       </c>
       <c r="V167" t="n">
+        <v>-0.03648619853180068</v>
+      </c>
+      <c r="W167" t="n">
         <v>30.68401387256897</v>
       </c>
     </row>
@@ -13875,6 +14378,9 @@
         </is>
       </c>
       <c r="V168" t="n">
+        <v>-0.00988979869153927</v>
+      </c>
+      <c r="W168" t="n">
         <v>35.69380741639211</v>
       </c>
     </row>
@@ -13955,6 +14461,9 @@
         </is>
       </c>
       <c r="V169" t="n">
+        <v>-0.01644216949653326</v>
+      </c>
+      <c r="W169" t="n">
         <v>35.11201430075555</v>
       </c>
     </row>
@@ -14035,6 +14544,9 @@
         </is>
       </c>
       <c r="V170" t="n">
+        <v>-0.03244108112499367</v>
+      </c>
+      <c r="W170" t="n">
         <v>32.00485992472102</v>
       </c>
     </row>
@@ -14115,6 +14627,9 @@
         </is>
       </c>
       <c r="V171" t="n">
+        <v>-0.04617461034197268</v>
+      </c>
+      <c r="W171" t="n">
         <v>28.69560806045617</v>
       </c>
     </row>
@@ -14195,6 +14710,9 @@
         </is>
       </c>
       <c r="V172" t="n">
+        <v>-0.01907883843746446</v>
+      </c>
+      <c r="W172" t="n">
         <v>33.91109645194221</v>
       </c>
     </row>
@@ -14275,6 +14793,9 @@
         </is>
       </c>
       <c r="V173" t="n">
+        <v>0.1118926792608279</v>
+      </c>
+      <c r="W173" t="n">
         <v>60.21566656616413</v>
       </c>
     </row>
@@ -14355,6 +14876,9 @@
         </is>
       </c>
       <c r="V174" t="n">
+        <v>-0.02596958651195092</v>
+      </c>
+      <c r="W174" t="n">
         <v>33.4102237290627</v>
       </c>
     </row>
@@ -14435,6 +14959,9 @@
         </is>
       </c>
       <c r="V175" t="n">
+        <v>-0.005113169489411464</v>
+      </c>
+      <c r="W175" t="n">
         <v>38.03194460326063</v>
       </c>
     </row>
@@ -14515,6 +15042,9 @@
         </is>
       </c>
       <c r="V176" t="n">
+        <v>-0.008832141837422888</v>
+      </c>
+      <c r="W176" t="n">
         <v>35.92978347953776</v>
       </c>
     </row>
@@ -14595,6 +15125,9 @@
         </is>
       </c>
       <c r="V177" t="n">
+        <v>-0.05659778036841038</v>
+      </c>
+      <c r="W177" t="n">
         <v>24.16620978835859</v>
       </c>
     </row>
@@ -14675,6 +15208,9 @@
         </is>
       </c>
       <c r="V178" t="n">
+        <v>-0.02387101399806946</v>
+      </c>
+      <c r="W178" t="n">
         <v>33.16308066817385</v>
       </c>
     </row>
@@ -14755,6 +15291,9 @@
         </is>
       </c>
       <c r="V179" t="n">
+        <v>-0.04308449639964562</v>
+      </c>
+      <c r="W179" t="n">
         <v>28.82876653943536</v>
       </c>
     </row>
@@ -14835,6 +15374,9 @@
         </is>
       </c>
       <c r="V180" t="n">
+        <v>-0.004188316060556319</v>
+      </c>
+      <c r="W180" t="n">
         <v>34.50807634052089</v>
       </c>
     </row>
@@ -14915,6 +15457,9 @@
         </is>
       </c>
       <c r="V181" t="n">
+        <v>-0.02940027546334526</v>
+      </c>
+      <c r="W181" t="n">
         <v>32.67880630995674</v>
       </c>
     </row>
@@ -14995,6 +15540,9 @@
         </is>
       </c>
       <c r="V182" t="n">
+        <v>-0.02111887944172099</v>
+      </c>
+      <c r="W182" t="n">
         <v>34.2349544588233</v>
       </c>
     </row>
@@ -15075,6 +15623,9 @@
         </is>
       </c>
       <c r="V183" t="n">
+        <v>-0.04165154368141493</v>
+      </c>
+      <c r="W183" t="n">
         <v>29.94868919070915</v>
       </c>
     </row>
@@ -15155,6 +15706,9 @@
         </is>
       </c>
       <c r="V184" t="n">
+        <v>-0.01828254858595958</v>
+      </c>
+      <c r="W184" t="n">
         <v>34.73201328301565</v>
       </c>
     </row>
@@ -15235,6 +15789,9 @@
         </is>
       </c>
       <c r="V185" t="n">
+        <v>-0.02647734803830993</v>
+      </c>
+      <c r="W185" t="n">
         <v>32.89239006344319</v>
       </c>
     </row>
@@ -15315,6 +15872,9 @@
         </is>
       </c>
       <c r="V186" t="n">
+        <v>-0.0246755438341988</v>
+      </c>
+      <c r="W186" t="n">
         <v>32.94772839050088</v>
       </c>
     </row>
@@ -15395,6 +15955,9 @@
         </is>
       </c>
       <c r="V187" t="n">
+        <v>-0.02882064826829041</v>
+      </c>
+      <c r="W187" t="n">
         <v>32.42374220716517</v>
       </c>
     </row>
@@ -15475,6 +16038,9 @@
         </is>
       </c>
       <c r="V188" t="n">
+        <v>-0.009877386765881086</v>
+      </c>
+      <c r="W188" t="n">
         <v>35.89545309716427</v>
       </c>
     </row>
@@ -15555,6 +16121,9 @@
         </is>
       </c>
       <c r="V189" t="n">
+        <v>-0.03531454518845444</v>
+      </c>
+      <c r="W189" t="n">
         <v>31.67846171294505</v>
       </c>
     </row>
@@ -15635,6 +16204,9 @@
         </is>
       </c>
       <c r="V190" t="n">
+        <v>-0.02542950725723505</v>
+      </c>
+      <c r="W190" t="n">
         <v>33.63044269730031</v>
       </c>
     </row>
@@ -15715,6 +16287,9 @@
         </is>
       </c>
       <c r="V191" t="n">
+        <v>0.003600615966581233</v>
+      </c>
+      <c r="W191" t="n">
         <v>33.97025373845899</v>
       </c>
     </row>
@@ -15795,6 +16370,9 @@
         </is>
       </c>
       <c r="V192" t="n">
+        <v>-0.001457525553647347</v>
+      </c>
+      <c r="W192" t="n">
         <v>32.98241443939305</v>
       </c>
     </row>
@@ -15875,6 +16453,9 @@
         </is>
       </c>
       <c r="V193" t="n">
+        <v>-0.05481807858931986</v>
+      </c>
+      <c r="W193" t="n">
         <v>27.13134606122544</v>
       </c>
     </row>
@@ -15955,6 +16536,9 @@
         </is>
       </c>
       <c r="V194" t="n">
+        <v>-0.06410257178274333</v>
+      </c>
+      <c r="W194" t="n">
         <v>22.81635371364017</v>
       </c>
     </row>
@@ -16035,6 +16619,9 @@
         </is>
       </c>
       <c r="V195" t="n">
+        <v>-0.05362065812309443</v>
+      </c>
+      <c r="W195" t="n">
         <v>24.32259088127175</v>
       </c>
     </row>
@@ -16115,6 +16702,9 @@
         </is>
       </c>
       <c r="V196" t="n">
+        <v>0.0193206181940537</v>
+      </c>
+      <c r="W196" t="n">
         <v>39.58057938790786</v>
       </c>
     </row>
@@ -16195,6 +16785,9 @@
         </is>
       </c>
       <c r="V197" t="n">
+        <v>-0.01238172539548517</v>
+      </c>
+      <c r="W197" t="n">
         <v>36.29539247184358</v>
       </c>
     </row>
@@ -16275,6 +16868,9 @@
         </is>
       </c>
       <c r="V198" t="n">
+        <v>-0.02852536575209957</v>
+      </c>
+      <c r="W198" t="n">
         <v>32.53055992287051</v>
       </c>
     </row>
@@ -16355,6 +16951,9 @@
         </is>
       </c>
       <c r="V199" t="n">
+        <v>0.06106510925101933</v>
+      </c>
+      <c r="W199" t="n">
         <v>34.82796668126873</v>
       </c>
     </row>
@@ -16435,6 +17034,9 @@
         </is>
       </c>
       <c r="V200" t="n">
+        <v>-0.08662455617140125</v>
+      </c>
+      <c r="W200" t="n">
         <v>15.96893911031469</v>
       </c>
     </row>
@@ -16515,6 +17117,9 @@
         </is>
       </c>
       <c r="V201" t="n">
+        <v>-0.008705464509657984</v>
+      </c>
+      <c r="W201" t="n">
         <v>35.3441370312732</v>
       </c>
     </row>
@@ -16595,6 +17200,9 @@
         </is>
       </c>
       <c r="V202" t="n">
+        <v>-0.01311758704299844</v>
+      </c>
+      <c r="W202" t="n">
         <v>35.36323891249854</v>
       </c>
     </row>
@@ -16675,6 +17283,9 @@
         </is>
       </c>
       <c r="V203" t="n">
+        <v>-0.01955144619666009</v>
+      </c>
+      <c r="W203" t="n">
         <v>34.49865577361162</v>
       </c>
     </row>
@@ -16755,6 +17366,9 @@
         </is>
       </c>
       <c r="V204" t="n">
+        <v>0.01465579921917403</v>
+      </c>
+      <c r="W204" t="n">
         <v>40.37142152643501</v>
       </c>
     </row>
@@ -16835,6 +17449,9 @@
         </is>
       </c>
       <c r="V205" t="n">
+        <v>-0.06380512028296802</v>
+      </c>
+      <c r="W205" t="n">
         <v>19.95067663918272</v>
       </c>
     </row>
@@ -16915,6 +17532,9 @@
         </is>
       </c>
       <c r="V206" t="n">
+        <v>-0.02216617784703468</v>
+      </c>
+      <c r="W206" t="n">
         <v>29.92013049131037</v>
       </c>
     </row>
@@ -16995,6 +17615,9 @@
         </is>
       </c>
       <c r="V207" t="n">
+        <v>-0.01742941373164737</v>
+      </c>
+      <c r="W207" t="n">
         <v>33.71697216821157</v>
       </c>
     </row>
@@ -17075,6 +17698,9 @@
         </is>
       </c>
       <c r="V208" t="n">
+        <v>-0.03877674236397451</v>
+      </c>
+      <c r="W208" t="n">
         <v>28.88981006757153</v>
       </c>
     </row>
@@ -17155,6 +17781,9 @@
         </is>
       </c>
       <c r="V209" t="n">
+        <v>-0.06983358291800799</v>
+      </c>
+      <c r="W209" t="n">
         <v>23.81755750817018</v>
       </c>
     </row>
@@ -17235,6 +17864,9 @@
         </is>
       </c>
       <c r="V210" t="n">
+        <v>-0.03242101274100132</v>
+      </c>
+      <c r="W210" t="n">
         <v>30.8208255539135</v>
       </c>
     </row>
@@ -17315,6 +17947,9 @@
         </is>
       </c>
       <c r="V211" t="n">
+        <v>-0.02262992416906051</v>
+      </c>
+      <c r="W211" t="n">
         <v>33.31401090642564</v>
       </c>
     </row>
@@ -17395,6 +18030,9 @@
         </is>
       </c>
       <c r="V212" t="n">
+        <v>-0.01657514977219367</v>
+      </c>
+      <c r="W212" t="n">
         <v>33.85528167299726</v>
       </c>
     </row>
@@ -17475,6 +18113,9 @@
         </is>
       </c>
       <c r="V213" t="n">
+        <v>-0.00397576167462798</v>
+      </c>
+      <c r="W213" t="n">
         <v>36.14616137409469</v>
       </c>
     </row>
@@ -17555,6 +18196,9 @@
         </is>
       </c>
       <c r="V214" t="n">
+        <v>-0.03755086965429687</v>
+      </c>
+      <c r="W214" t="n">
         <v>30.52839377998344</v>
       </c>
     </row>
@@ -17635,6 +18279,9 @@
         </is>
       </c>
       <c r="V215" t="n">
+        <v>-0.03308927779590858</v>
+      </c>
+      <c r="W215" t="n">
         <v>31.13058065650155</v>
       </c>
     </row>
@@ -17715,6 +18362,9 @@
         </is>
       </c>
       <c r="V216" t="n">
+        <v>-0.0537078135285147</v>
+      </c>
+      <c r="W216" t="n">
         <v>25.20233694622018</v>
       </c>
     </row>
@@ -17795,6 +18445,9 @@
         </is>
       </c>
       <c r="V217" t="n">
+        <v>-0.04437556516985292</v>
+      </c>
+      <c r="W217" t="n">
         <v>28.16910717939869</v>
       </c>
     </row>
@@ -17875,6 +18528,9 @@
         </is>
       </c>
       <c r="V218" t="n">
+        <v>0.0102601194398276</v>
+      </c>
+      <c r="W218" t="n">
         <v>37.96618265481536</v>
       </c>
     </row>
@@ -17955,6 +18611,9 @@
         </is>
       </c>
       <c r="V219" t="n">
+        <v>-0.03770552319960783</v>
+      </c>
+      <c r="W219" t="n">
         <v>30.49369805288224</v>
       </c>
     </row>
@@ -18035,6 +18694,9 @@
         </is>
       </c>
       <c r="V220" t="n">
+        <v>-0.007715658424359474</v>
+      </c>
+      <c r="W220" t="n">
         <v>36.63236173975828</v>
       </c>
     </row>
@@ -18115,6 +18777,9 @@
         </is>
       </c>
       <c r="V221" t="n">
+        <v>-0.04082394645896859</v>
+      </c>
+      <c r="W221" t="n">
         <v>29.34927884196232</v>
       </c>
     </row>
@@ -18195,6 +18860,9 @@
         </is>
       </c>
       <c r="V222" t="n">
+        <v>0.01114135110854774</v>
+      </c>
+      <c r="W222" t="n">
         <v>39.76147058055393</v>
       </c>
     </row>
@@ -18275,6 +18943,9 @@
         </is>
       </c>
       <c r="V223" t="n">
+        <v>-0.03960994453303025</v>
+      </c>
+      <c r="W223" t="n">
         <v>29.79511256930715</v>
       </c>
     </row>
@@ -18355,6 +19026,9 @@
         </is>
       </c>
       <c r="V224" t="n">
+        <v>0.03092846821605257</v>
+      </c>
+      <c r="W224" t="n">
         <v>41.17775721480717</v>
       </c>
     </row>
@@ -18435,6 +19109,9 @@
         </is>
       </c>
       <c r="V225" t="n">
+        <v>-0.03516526901577017</v>
+      </c>
+      <c r="W225" t="n">
         <v>30.05178588019956</v>
       </c>
     </row>
@@ -18515,6 +19192,9 @@
         </is>
       </c>
       <c r="V226" t="n">
+        <v>-0.0275073212755053</v>
+      </c>
+      <c r="W226" t="n">
         <v>32.27452798910134</v>
       </c>
     </row>
@@ -18595,6 +19275,9 @@
         </is>
       </c>
       <c r="V227" t="n">
+        <v>-0.04200547094832707</v>
+      </c>
+      <c r="W227" t="n">
         <v>30.44170948270091</v>
       </c>
     </row>
@@ -18675,6 +19358,9 @@
         </is>
       </c>
       <c r="V228" t="n">
+        <v>-0.04044521328253161</v>
+      </c>
+      <c r="W228" t="n">
         <v>29.08699810858241</v>
       </c>
     </row>
@@ -18755,6 +19441,9 @@
         </is>
       </c>
       <c r="V229" t="n">
+        <v>-0.02188728288911957</v>
+      </c>
+      <c r="W229" t="n">
         <v>33.02062788004914</v>
       </c>
     </row>
@@ -18835,6 +19524,9 @@
         </is>
       </c>
       <c r="V230" t="n">
+        <v>-0.01276482806421362</v>
+      </c>
+      <c r="W230" t="n">
         <v>36.28835399701841</v>
       </c>
     </row>
@@ -18915,6 +19607,9 @@
         </is>
       </c>
       <c r="V231" t="n">
+        <v>-0.01128616310984422</v>
+      </c>
+      <c r="W231" t="n">
         <v>36.42434756694555</v>
       </c>
     </row>
@@ -18995,6 +19690,9 @@
         </is>
       </c>
       <c r="V232" t="n">
+        <v>-0.0287234780588656</v>
+      </c>
+      <c r="W232" t="n">
         <v>31.47788307838973</v>
       </c>
     </row>
@@ -19075,6 +19773,9 @@
         </is>
       </c>
       <c r="V233" t="n">
+        <v>-0.03517807227469038</v>
+      </c>
+      <c r="W233" t="n">
         <v>30.79499038101841</v>
       </c>
     </row>
@@ -19155,6 +19856,9 @@
         </is>
       </c>
       <c r="V234" t="n">
+        <v>-0.0295678335329096</v>
+      </c>
+      <c r="W234" t="n">
         <v>32.46905299713534</v>
       </c>
     </row>
@@ -19235,6 +19939,9 @@
         </is>
       </c>
       <c r="V235" t="n">
+        <v>-0.05316400082564488</v>
+      </c>
+      <c r="W235" t="n">
         <v>26.11844263748779</v>
       </c>
     </row>
@@ -19315,6 +20022,9 @@
         </is>
       </c>
       <c r="V236" t="n">
+        <v>-0.02752670743566825</v>
+      </c>
+      <c r="W236" t="n">
         <v>32.86144112532298</v>
       </c>
     </row>
@@ -19395,6 +20105,9 @@
         </is>
       </c>
       <c r="V237" t="n">
+        <v>-0.02839830316077111</v>
+      </c>
+      <c r="W237" t="n">
         <v>32.02866539244578</v>
       </c>
     </row>
@@ -19475,6 +20188,9 @@
         </is>
       </c>
       <c r="V238" t="n">
+        <v>0.01609188320772943</v>
+      </c>
+      <c r="W238" t="n">
         <v>40.04755095665013</v>
       </c>
     </row>
@@ -19555,6 +20271,9 @@
         </is>
       </c>
       <c r="V239" t="n">
+        <v>-0.00304053255929935</v>
+      </c>
+      <c r="W239" t="n">
         <v>38.10447511541902</v>
       </c>
     </row>
@@ -19635,6 +20354,9 @@
         </is>
       </c>
       <c r="V240" t="n">
+        <v>-0.02751475724983871</v>
+      </c>
+      <c r="W240" t="n">
         <v>31.44971841689833</v>
       </c>
     </row>
@@ -19715,6 +20437,9 @@
         </is>
       </c>
       <c r="V241" t="n">
+        <v>-0.03055293108791476</v>
+      </c>
+      <c r="W241" t="n">
         <v>32.08987514772272</v>
       </c>
     </row>
@@ -19795,6 +20520,9 @@
         </is>
       </c>
       <c r="V242" t="n">
+        <v>0.1994632120973422</v>
+      </c>
+      <c r="W242" t="n">
         <v>65.4090344358751</v>
       </c>
     </row>
@@ -19875,6 +20603,9 @@
         </is>
       </c>
       <c r="V243" t="n">
+        <v>-0.04663369930193437</v>
+      </c>
+      <c r="W243" t="n">
         <v>25.29355523094111</v>
       </c>
     </row>
@@ -19955,6 +20686,9 @@
         </is>
       </c>
       <c r="V244" t="n">
+        <v>-0.03063391776119758</v>
+      </c>
+      <c r="W244" t="n">
         <v>31.77888063887504</v>
       </c>
     </row>
@@ -20035,6 +20769,9 @@
         </is>
       </c>
       <c r="V245" t="n">
+        <v>-0.07344368409280973</v>
+      </c>
+      <c r="W245" t="n">
         <v>18.91249969717309</v>
       </c>
     </row>
@@ -20115,6 +20852,9 @@
         </is>
       </c>
       <c r="V246" t="n">
+        <v>-0.02386249326864197</v>
+      </c>
+      <c r="W246" t="n">
         <v>34.37788891864695</v>
       </c>
     </row>
@@ -20195,6 +20935,9 @@
         </is>
       </c>
       <c r="V247" t="n">
+        <v>-0.03812186413146574</v>
+      </c>
+      <c r="W247" t="n">
         <v>28.90741060695267</v>
       </c>
     </row>
@@ -20275,6 +21018,9 @@
         </is>
       </c>
       <c r="V248" t="n">
+        <v>-0.009889667041823584</v>
+      </c>
+      <c r="W248" t="n">
         <v>34.88245620048065</v>
       </c>
     </row>
@@ -20355,6 +21101,9 @@
         </is>
       </c>
       <c r="V249" t="n">
+        <v>-0.05247805136896818</v>
+      </c>
+      <c r="W249" t="n">
         <v>26.21366515516785</v>
       </c>
     </row>
@@ -20435,6 +21184,9 @@
         </is>
       </c>
       <c r="V250" t="n">
+        <v>-0.0266143701468392</v>
+      </c>
+      <c r="W250" t="n">
         <v>32.73613013048766</v>
       </c>
     </row>
@@ -20515,6 +21267,9 @@
         </is>
       </c>
       <c r="V251" t="n">
+        <v>-0.01169500965710967</v>
+      </c>
+      <c r="W251" t="n">
         <v>36.32173016376302</v>
       </c>
     </row>
@@ -20595,6 +21350,9 @@
         </is>
       </c>
       <c r="V252" t="n">
+        <v>0.004192612818547568</v>
+      </c>
+      <c r="W252" t="n">
         <v>36.46153814438935</v>
       </c>
     </row>
@@ -20675,6 +21433,9 @@
         </is>
       </c>
       <c r="V253" t="n">
+        <v>-0.01920944666267459</v>
+      </c>
+      <c r="W253" t="n">
         <v>34.94472052810271</v>
       </c>
     </row>
@@ -20755,6 +21516,9 @@
         </is>
       </c>
       <c r="V254" t="n">
+        <v>-0.04396210375727544</v>
+      </c>
+      <c r="W254" t="n">
         <v>28.24814781039276</v>
       </c>
     </row>
@@ -20835,6 +21599,9 @@
         </is>
       </c>
       <c r="V255" t="n">
+        <v>-0.02359996107963849</v>
+      </c>
+      <c r="W255" t="n">
         <v>34.19969406457524</v>
       </c>
     </row>
@@ -20915,6 +21682,9 @@
         </is>
       </c>
       <c r="V256" t="n">
+        <v>-0.03079883747949573</v>
+      </c>
+      <c r="W256" t="n">
         <v>31.64060261127175</v>
       </c>
     </row>
@@ -20995,6 +21765,9 @@
         </is>
       </c>
       <c r="V257" t="n">
+        <v>-0.01767788667965128</v>
+      </c>
+      <c r="W257" t="n">
         <v>34.22377668431979</v>
       </c>
     </row>
@@ -21075,6 +21848,9 @@
         </is>
       </c>
       <c r="V258" t="n">
+        <v>-0.02988565522958402</v>
+      </c>
+      <c r="W258" t="n">
         <v>31.5636151542142</v>
       </c>
     </row>
@@ -21155,6 +21931,9 @@
         </is>
       </c>
       <c r="V259" t="n">
+        <v>0.01585626341576416</v>
+      </c>
+      <c r="W259" t="n">
         <v>41.29104752220794</v>
       </c>
     </row>
@@ -21235,6 +22014,9 @@
         </is>
       </c>
       <c r="V260" t="n">
+        <v>-0.0207922139459165</v>
+      </c>
+      <c r="W260" t="n">
         <v>34.0940699461401</v>
       </c>
     </row>
@@ -21315,6 +22097,9 @@
         </is>
       </c>
       <c r="V261" t="n">
+        <v>-0.002880618503153985</v>
+      </c>
+      <c r="W261" t="n">
         <v>37.55666325649182</v>
       </c>
     </row>
@@ -21395,6 +22180,9 @@
         </is>
       </c>
       <c r="V262" t="n">
+        <v>-0.01931705475497852</v>
+      </c>
+      <c r="W262" t="n">
         <v>34.60486485845527</v>
       </c>
     </row>
@@ -21475,6 +22263,9 @@
         </is>
       </c>
       <c r="V263" t="n">
+        <v>-0.0208606259549939</v>
+      </c>
+      <c r="W263" t="n">
         <v>31.61834330448933</v>
       </c>
     </row>
@@ -21555,6 +22346,9 @@
         </is>
       </c>
       <c r="V264" t="n">
+        <v>-0.005731626638565167</v>
+      </c>
+      <c r="W264" t="n">
         <v>34.05744407761883</v>
       </c>
     </row>
@@ -21635,6 +22429,9 @@
         </is>
       </c>
       <c r="V265" t="n">
+        <v>-0.04633456938681019</v>
+      </c>
+      <c r="W265" t="n">
         <v>27.83381676380894</v>
       </c>
     </row>
@@ -21715,6 +22512,9 @@
         </is>
       </c>
       <c r="V266" t="n">
+        <v>-0.02317533386011708</v>
+      </c>
+      <c r="W266" t="n">
         <v>33.22680596698528</v>
       </c>
     </row>
@@ -21795,6 +22595,9 @@
         </is>
       </c>
       <c r="V267" t="n">
+        <v>-0.04529113534213297</v>
+      </c>
+      <c r="W267" t="n">
         <v>27.91302386042464</v>
       </c>
     </row>
@@ -21875,6 +22678,9 @@
         </is>
       </c>
       <c r="V268" t="n">
+        <v>-0.03738061937405997</v>
+      </c>
+      <c r="W268" t="n">
         <v>29.95182158254128</v>
       </c>
     </row>
@@ -21955,6 +22761,9 @@
         </is>
       </c>
       <c r="V269" t="n">
+        <v>-0.0264291854957057</v>
+      </c>
+      <c r="W269" t="n">
         <v>31.9821855012566</v>
       </c>
     </row>
@@ -22035,6 +22844,9 @@
         </is>
       </c>
       <c r="V270" t="n">
+        <v>-0.04036128828002452</v>
+      </c>
+      <c r="W270" t="n">
         <v>29.14025919122388</v>
       </c>
     </row>
@@ -22115,6 +22927,9 @@
         </is>
       </c>
       <c r="V271" t="n">
+        <v>-0.067976987227356</v>
+      </c>
+      <c r="W271" t="n">
         <v>24.34674295272591</v>
       </c>
     </row>
@@ -22195,6 +23010,9 @@
         </is>
       </c>
       <c r="V272" t="n">
+        <v>-0.02231292282577077</v>
+      </c>
+      <c r="W272" t="n">
         <v>34.98341035590214</v>
       </c>
     </row>
@@ -22275,6 +23093,9 @@
         </is>
       </c>
       <c r="V273" t="n">
+        <v>-0.03298839822316191</v>
+      </c>
+      <c r="W273" t="n">
         <v>30.17295386048777</v>
       </c>
     </row>
@@ -22355,6 +23176,9 @@
         </is>
       </c>
       <c r="V274" t="n">
+        <v>-0.02273719036719601</v>
+      </c>
+      <c r="W274" t="n">
         <v>34.0725853781528</v>
       </c>
     </row>
@@ -22435,6 +23259,9 @@
         </is>
       </c>
       <c r="V275" t="n">
+        <v>-0.0228231134136994</v>
+      </c>
+      <c r="W275" t="n">
         <v>34.28432760481187</v>
       </c>
     </row>
@@ -22515,6 +23342,9 @@
         </is>
       </c>
       <c r="V276" t="n">
+        <v>-0.08406414823419277</v>
+      </c>
+      <c r="W276" t="n">
         <v>12.41554472742747</v>
       </c>
     </row>
@@ -22595,6 +23425,9 @@
         </is>
       </c>
       <c r="V277" t="n">
+        <v>-0.02623870675780129</v>
+      </c>
+      <c r="W277" t="n">
         <v>32.96645339081318</v>
       </c>
     </row>
@@ -22675,6 +23508,9 @@
         </is>
       </c>
       <c r="V278" t="n">
+        <v>-0.01865313216588569</v>
+      </c>
+      <c r="W278" t="n">
         <v>34.32817961152141</v>
       </c>
     </row>
@@ -22755,6 +23591,9 @@
         </is>
       </c>
       <c r="V279" t="n">
+        <v>-0.03906331702109671</v>
+      </c>
+      <c r="W279" t="n">
         <v>29.57794457987779</v>
       </c>
     </row>
@@ -22835,6 +23674,9 @@
         </is>
       </c>
       <c r="V280" t="n">
+        <v>-0.04830500916842228</v>
+      </c>
+      <c r="W280" t="n">
         <v>26.70340813585858</v>
       </c>
     </row>
@@ -22915,6 +23757,9 @@
         </is>
       </c>
       <c r="V281" t="n">
+        <v>-0.03255673602257186</v>
+      </c>
+      <c r="W281" t="n">
         <v>32.18955303654384</v>
       </c>
     </row>
@@ -22995,6 +23840,9 @@
         </is>
       </c>
       <c r="V282" t="n">
+        <v>-0.03644338648707154</v>
+      </c>
+      <c r="W282" t="n">
         <v>31.0694059489477</v>
       </c>
     </row>
@@ -23075,6 +23923,9 @@
         </is>
       </c>
       <c r="V283" t="n">
+        <v>-0.009798579793105633</v>
+      </c>
+      <c r="W283" t="n">
         <v>31.07542570715927</v>
       </c>
     </row>
@@ -23155,6 +24006,9 @@
         </is>
       </c>
       <c r="V284" t="n">
+        <v>-0.01835046594859003</v>
+      </c>
+      <c r="W284" t="n">
         <v>35.39094027825132</v>
       </c>
     </row>
@@ -23235,6 +24089,9 @@
         </is>
       </c>
       <c r="V285" t="n">
+        <v>0.01849299127217318</v>
+      </c>
+      <c r="W285" t="n">
         <v>37.12925780595957</v>
       </c>
     </row>
@@ -23315,6 +24172,9 @@
         </is>
       </c>
       <c r="V286" t="n">
+        <v>-0.0646746990789292</v>
+      </c>
+      <c r="W286" t="n">
         <v>22.9458521855127</v>
       </c>
     </row>
@@ -23395,6 +24255,9 @@
         </is>
       </c>
       <c r="V287" t="n">
+        <v>-0.01827276004698613</v>
+      </c>
+      <c r="W287" t="n">
         <v>34.96125007361939</v>
       </c>
     </row>
@@ -23475,6 +24338,9 @@
         </is>
       </c>
       <c r="V288" t="n">
+        <v>-0.03734909014500554</v>
+      </c>
+      <c r="W288" t="n">
         <v>29.10363354850589</v>
       </c>
     </row>
@@ -23555,6 +24421,9 @@
         </is>
       </c>
       <c r="V289" t="n">
+        <v>-0.02714802558596018</v>
+      </c>
+      <c r="W289" t="n">
         <v>32.53175290365366</v>
       </c>
     </row>
@@ -23635,6 +24504,9 @@
         </is>
       </c>
       <c r="V290" t="n">
+        <v>-0.02802969736520524</v>
+      </c>
+      <c r="W290" t="n">
         <v>32.82520883850695</v>
       </c>
     </row>
@@ -23715,6 +24587,9 @@
         </is>
       </c>
       <c r="V291" t="n">
+        <v>-0.03893026409366943</v>
+      </c>
+      <c r="W291" t="n">
         <v>30.38788647284481</v>
       </c>
     </row>

</xml_diff>